<commit_message>
limma removeBatchEffect, GO analysis, updating Figures 1 and 2
</commit_message>
<xml_diff>
--- a/physiology/4_R_intensity/data_rscores.xlsx
+++ b/physiology/4_R_intensity/data_rscores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_temperaturevariability2023/physiology/R_intensity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miamiedu-my.sharepoint.com/personal/and128_miami_edu/Documents/GitHub/Ch2_temperaturevariability2023/physiology/4_R_intensity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="14_{35844A45-6BE5-1345-9C52-0F5E191FDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF70052D-9B2C-214C-A248-3A45E19FC359}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="14_{35844A45-6BE5-1345-9C52-0F5E191FDADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08F6B122-2223-A549-8767-B1EC66855EDA}"/>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="500" windowWidth="15060" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13740" yWindow="500" windowWidth="15060" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_rscores" sheetId="1" r:id="rId1"/>
@@ -603,14 +603,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -648,7 +644,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -754,7 +750,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -896,7 +892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -908,7 +904,7 @@
   <dimension ref="A1:G3369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1942" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2950" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1961" sqref="B1961"/>
     </sheetView>
   </sheetViews>
@@ -61657,7 +61653,7 @@
         <v>2261.5</v>
       </c>
     </row>
-    <row r="2642" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2642" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2642" s="1">
         <v>44750</v>
       </c>
@@ -61680,7 +61676,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="2643" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2643" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2643" s="1">
         <v>44750</v>
       </c>
@@ -61703,7 +61699,7 @@
         <v>2135.1669999999999</v>
       </c>
     </row>
-    <row r="2644" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2644" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2644" s="1">
         <v>44750</v>
       </c>
@@ -61726,7 +61722,7 @@
         <v>2125.8330000000001</v>
       </c>
     </row>
-    <row r="2645" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2645" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2645" s="1">
         <v>44750</v>
       </c>
@@ -61749,7 +61745,7 @@
         <v>2119.1669999999999</v>
       </c>
     </row>
-    <row r="2646" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2646" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2646" s="1">
         <v>44750</v>
       </c>
@@ -61772,7 +61768,7 @@
         <v>2081.5</v>
       </c>
     </row>
-    <row r="2647" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2647" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2647" s="1">
         <v>44750</v>
       </c>
@@ -61795,7 +61791,7 @@
         <v>2068.1669999999999</v>
       </c>
     </row>
-    <row r="2648" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2648" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2648" s="1">
         <v>44750</v>
       </c>
@@ -61818,7 +61814,7 @@
         <v>2073.5</v>
       </c>
     </row>
-    <row r="2649" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2649" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2649" s="1">
         <v>44750</v>
       </c>
@@ -61841,7 +61837,7 @@
         <v>2070.8330000000001</v>
       </c>
     </row>
-    <row r="2650" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2650" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2650" s="1">
         <v>44750</v>
       </c>
@@ -61864,7 +61860,7 @@
         <v>2152.5</v>
       </c>
     </row>
-    <row r="2651" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2651" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2651" s="1">
         <v>44750</v>
       </c>
@@ -61887,7 +61883,7 @@
         <v>2130.5</v>
       </c>
     </row>
-    <row r="2652" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2652" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2652" s="1">
         <v>44750</v>
       </c>
@@ -61910,7 +61906,7 @@
         <v>2132.5</v>
       </c>
     </row>
-    <row r="2653" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2653" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2653" s="1">
         <v>44750</v>
       </c>
@@ -61933,7 +61929,7 @@
         <v>2138.5</v>
       </c>
     </row>
-    <row r="2654" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2654" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2654" s="1">
         <v>44750</v>
       </c>
@@ -61956,7 +61952,7 @@
         <v>2234.5</v>
       </c>
     </row>
-    <row r="2655" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2655" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2655" s="1">
         <v>44750</v>
       </c>
@@ -61979,7 +61975,7 @@
         <v>2202.5</v>
       </c>
     </row>
-    <row r="2656" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2656" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2656" s="1">
         <v>44750</v>
       </c>
@@ -62002,7 +61998,7 @@
         <v>2198.5</v>
       </c>
     </row>
-    <row r="2657" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2657" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2657" s="1">
         <v>44750</v>
       </c>
@@ -62025,7 +62021,7 @@
         <v>2180.5</v>
       </c>
     </row>
-    <row r="2658" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2658" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2658" s="1">
         <v>44750</v>
       </c>
@@ -62048,7 +62044,7 @@
         <v>2213.5</v>
       </c>
     </row>
-    <row r="2659" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2659" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2659" s="1">
         <v>44750</v>
       </c>
@@ -62071,7 +62067,7 @@
         <v>2233.5</v>
       </c>
     </row>
-    <row r="2660" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2660" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2660" s="1">
         <v>44750</v>
       </c>
@@ -62094,7 +62090,7 @@
         <v>2241.5</v>
       </c>
     </row>
-    <row r="2661" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2661" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2661" s="1">
         <v>44750</v>
       </c>
@@ -62117,7 +62113,7 @@
         <v>2231.5</v>
       </c>
     </row>
-    <row r="2662" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2662" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2662" s="1">
         <v>44750</v>
       </c>
@@ -62140,7 +62136,7 @@
         <v>2115.5</v>
       </c>
     </row>
-    <row r="2663" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2663" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2663" s="1">
         <v>44750</v>
       </c>
@@ -62163,7 +62159,7 @@
         <v>2117.5</v>
       </c>
     </row>
-    <row r="2664" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2664" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2664" s="1">
         <v>44750</v>
       </c>
@@ -62186,7 +62182,7 @@
         <v>2107.5</v>
       </c>
     </row>
-    <row r="2665" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2665" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2665" s="1">
         <v>44750</v>
       </c>
@@ -62209,7 +62205,7 @@
         <v>2097.5</v>
       </c>
     </row>
-    <row r="2666" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2666" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2666" s="1">
         <v>44750</v>
       </c>
@@ -62232,7 +62228,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="2667" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2667" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2667" s="1">
         <v>44750</v>
       </c>
@@ -62255,7 +62251,7 @@
         <v>2120.5</v>
       </c>
     </row>
-    <row r="2668" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2668" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2668" s="1">
         <v>44750</v>
       </c>
@@ -62278,7 +62274,7 @@
         <v>2116.5</v>
       </c>
     </row>
-    <row r="2669" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2669" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2669" s="1">
         <v>44750</v>
       </c>
@@ -62301,7 +62297,7 @@
         <v>2122.5</v>
       </c>
     </row>
-    <row r="2670" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2670" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2670" s="1">
         <v>44750</v>
       </c>
@@ -62324,7 +62320,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="2671" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2671" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2671" s="1">
         <v>44750</v>
       </c>
@@ -62347,7 +62343,7 @@
         <v>2043.1669999999999</v>
       </c>
     </row>
-    <row r="2672" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2672" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2672" s="1">
         <v>44750</v>
       </c>
@@ -62370,7 +62366,7 @@
         <v>2063.1669999999999</v>
       </c>
     </row>
-    <row r="2673" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2673" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2673" s="1">
         <v>44750</v>
       </c>
@@ -62393,7 +62389,7 @@
         <v>2080.5</v>
       </c>
     </row>
-    <row r="2674" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2674" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2674" s="1">
         <v>44750</v>
       </c>
@@ -62416,7 +62412,7 @@
         <v>2014.5</v>
       </c>
     </row>
-    <row r="2675" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2675" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2675" s="1">
         <v>44750</v>
       </c>
@@ -62439,7 +62435,7 @@
         <v>2086.5</v>
       </c>
     </row>
-    <row r="2676" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2676" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2676" s="1">
         <v>44750</v>
       </c>
@@ -62462,7 +62458,7 @@
         <v>2026.5</v>
       </c>
     </row>
-    <row r="2677" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2677" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2677" s="1">
         <v>44750</v>
       </c>
@@ -62485,7 +62481,7 @@
         <v>2040.5</v>
       </c>
     </row>
-    <row r="2678" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2678" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2678" s="1">
         <v>44750</v>
       </c>
@@ -62508,7 +62504,7 @@
         <v>2046.5</v>
       </c>
     </row>
-    <row r="2679" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2679" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2679" s="1">
         <v>44750</v>
       </c>
@@ -62531,7 +62527,7 @@
         <v>2010.5</v>
       </c>
     </row>
-    <row r="2680" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2680" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2680" s="1">
         <v>44750</v>
       </c>
@@ -62554,7 +62550,7 @@
         <v>1996.5</v>
       </c>
     </row>
-    <row r="2681" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2681" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2681" s="1">
         <v>44750</v>
       </c>
@@ -62577,7 +62573,7 @@
         <v>1978.5</v>
       </c>
     </row>
-    <row r="2682" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2682" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2682" s="1">
         <v>44750</v>
       </c>
@@ -62600,7 +62596,7 @@
         <v>2053.5</v>
       </c>
     </row>
-    <row r="2683" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2683" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2683" s="1">
         <v>44750</v>
       </c>
@@ -62623,7 +62619,7 @@
         <v>2029.5</v>
       </c>
     </row>
-    <row r="2684" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2684" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2684" s="1">
         <v>44750</v>
       </c>
@@ -62646,7 +62642,7 @@
         <v>2043.5</v>
       </c>
     </row>
-    <row r="2685" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2685" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2685" s="1">
         <v>44750</v>
       </c>
@@ -62669,7 +62665,7 @@
         <v>2065.5</v>
       </c>
     </row>
-    <row r="2686" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2686" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2686" s="1">
         <v>44750</v>
       </c>
@@ -62692,7 +62688,7 @@
         <v>2039.5</v>
       </c>
     </row>
-    <row r="2687" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2687" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2687" s="1">
         <v>44750</v>
       </c>
@@ -62715,7 +62711,7 @@
         <v>2057.5</v>
       </c>
     </row>
-    <row r="2688" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2688" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2688" s="1">
         <v>44750</v>
       </c>
@@ -62738,7 +62734,7 @@
         <v>2045.5</v>
       </c>
     </row>
-    <row r="2689" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2689" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2689" s="1">
         <v>44750</v>
       </c>
@@ -62761,7 +62757,7 @@
         <v>2072.5</v>
       </c>
     </row>
-    <row r="2690" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2690" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2690" s="1">
         <v>44750</v>
       </c>
@@ -62784,7 +62780,7 @@
         <v>2015.5</v>
       </c>
     </row>
-    <row r="2691" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2691" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2691" s="1">
         <v>44750</v>
       </c>
@@ -62807,7 +62803,7 @@
         <v>2012.5</v>
       </c>
     </row>
-    <row r="2692" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2692" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2692" s="1">
         <v>44750</v>
       </c>
@@ -62830,7 +62826,7 @@
         <v>2045.5</v>
       </c>
     </row>
-    <row r="2693" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2693" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2693" s="1">
         <v>44750</v>
       </c>
@@ -62853,7 +62849,7 @@
         <v>2087.5</v>
       </c>
     </row>
-    <row r="2694" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2694" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2694" s="1">
         <v>44750</v>
       </c>
@@ -62876,7 +62872,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="2695" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2695" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2695" s="1">
         <v>44750</v>
       </c>
@@ -62899,7 +62895,7 @@
         <v>1995.8330000000001</v>
       </c>
     </row>
-    <row r="2696" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2696" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2696" s="1">
         <v>44750</v>
       </c>
@@ -62922,7 +62918,7 @@
         <v>1974.5</v>
       </c>
     </row>
-    <row r="2697" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2697" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2697" s="1">
         <v>44750</v>
       </c>
@@ -62945,7 +62941,7 @@
         <v>2002.5</v>
       </c>
     </row>
-    <row r="2698" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2698" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2698" s="1">
         <v>44750</v>
       </c>
@@ -62968,7 +62964,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="2699" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2699" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2699" s="1">
         <v>44750</v>
       </c>
@@ -62991,7 +62987,7 @@
         <v>1730.5</v>
       </c>
     </row>
-    <row r="2700" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2700" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2700" s="1">
         <v>44750</v>
       </c>
@@ -63014,7 +63010,7 @@
         <v>1850.5</v>
       </c>
     </row>
-    <row r="2701" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2701" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2701" s="1">
         <v>44750</v>
       </c>
@@ -63037,7 +63033,7 @@
         <v>2028.5</v>
       </c>
     </row>
-    <row r="2702" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2702" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2702" s="1">
         <v>44750</v>
       </c>
@@ -63060,7 +63056,7 @@
         <v>1902.5</v>
       </c>
     </row>
-    <row r="2703" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2703" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2703" s="1">
         <v>44750</v>
       </c>
@@ -63083,7 +63079,7 @@
         <v>1976.5</v>
       </c>
     </row>
-    <row r="2704" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2704" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2704" s="1">
         <v>44750</v>
       </c>
@@ -63106,7 +63102,7 @@
         <v>2056.5</v>
       </c>
     </row>
-    <row r="2705" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2705" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2705" s="1">
         <v>44750</v>
       </c>
@@ -63129,7 +63125,7 @@
         <v>2122.5</v>
       </c>
     </row>
-    <row r="2706" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2706" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2706" s="1">
         <v>44750</v>
       </c>
@@ -63152,7 +63148,7 @@
         <v>1628.8330000000001</v>
       </c>
     </row>
-    <row r="2707" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2707" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2707" s="1">
         <v>44750</v>
       </c>
@@ -63175,7 +63171,7 @@
         <v>1819.5</v>
       </c>
     </row>
-    <row r="2708" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2708" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2708" s="1">
         <v>44750</v>
       </c>
@@ -63198,7 +63194,7 @@
         <v>1978.1669999999999</v>
       </c>
     </row>
-    <row r="2709" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2709" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2709" s="1">
         <v>44750</v>
       </c>
@@ -63221,7 +63217,7 @@
         <v>2078.1669999999999</v>
       </c>
     </row>
-    <row r="2710" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2710" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2710" s="1">
         <v>44750</v>
       </c>
@@ -63244,7 +63240,7 @@
         <v>1717.8330000000001</v>
       </c>
     </row>
-    <row r="2711" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2711" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2711" s="1">
         <v>44750</v>
       </c>
@@ -63267,7 +63263,7 @@
         <v>1711.1669999999999</v>
       </c>
     </row>
-    <row r="2712" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2712" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2712" s="1">
         <v>44750</v>
       </c>
@@ -63290,7 +63286,7 @@
         <v>2072.5</v>
       </c>
     </row>
-    <row r="2713" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2713" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2713" s="1">
         <v>44750</v>
       </c>
@@ -63313,7 +63309,7 @@
         <v>1975.5</v>
       </c>
     </row>
-    <row r="2714" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2714" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2714" s="1">
         <v>44750</v>
       </c>
@@ -63336,7 +63332,7 @@
         <v>1525.5</v>
       </c>
     </row>
-    <row r="2715" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2715" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2715" s="1">
         <v>44750</v>
       </c>
@@ -63359,7 +63355,7 @@
         <v>1703.5</v>
       </c>
     </row>
-    <row r="2716" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2716" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2716" s="1">
         <v>44750</v>
       </c>
@@ -63382,7 +63378,7 @@
         <v>1813.5</v>
       </c>
     </row>
-    <row r="2717" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2717" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2717" s="1">
         <v>44750</v>
       </c>
@@ -63405,7 +63401,7 @@
         <v>2049.5</v>
       </c>
     </row>
-    <row r="2718" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2718" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2718" s="1">
         <v>44750</v>
       </c>
@@ -63428,7 +63424,7 @@
         <v>1605.5</v>
       </c>
     </row>
-    <row r="2719" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2719" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2719" s="1">
         <v>44750</v>
       </c>
@@ -63451,7 +63447,7 @@
         <v>1703.5</v>
       </c>
     </row>
-    <row r="2720" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2720" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2720" s="1">
         <v>44750</v>
       </c>
@@ -63474,7 +63470,7 @@
         <v>1799.5</v>
       </c>
     </row>
-    <row r="2721" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2721" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2721" s="1">
         <v>44750</v>
       </c>
@@ -63497,7 +63493,7 @@
         <v>1941.5</v>
       </c>
     </row>
-    <row r="2722" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2722" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2722" s="1">
         <v>44750</v>
       </c>
@@ -63520,7 +63516,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="2723" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2723" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2723" s="1">
         <v>44750</v>
       </c>
@@ -63543,7 +63539,7 @@
         <v>1954.5</v>
       </c>
     </row>
-    <row r="2724" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2724" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2724" s="1">
         <v>44750</v>
       </c>
@@ -63566,7 +63562,7 @@
         <v>2043.8330000000001</v>
       </c>
     </row>
-    <row r="2725" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2725" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2725" s="1">
         <v>44750</v>
       </c>
@@ -63589,7 +63585,7 @@
         <v>2193.1669999999999</v>
       </c>
     </row>
-    <row r="2726" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2726" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2726" s="1">
         <v>44750</v>
       </c>
@@ -63612,7 +63608,7 @@
         <v>1642.5</v>
       </c>
     </row>
-    <row r="2727" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2727" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2727" s="1">
         <v>44750</v>
       </c>
@@ -63635,7 +63631,7 @@
         <v>1761.1669999999999</v>
       </c>
     </row>
-    <row r="2728" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2728" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2728" s="1">
         <v>44750</v>
       </c>
@@ -63658,7 +63654,7 @@
         <v>1874.5</v>
       </c>
     </row>
-    <row r="2729" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2729" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2729" s="1">
         <v>44750</v>
       </c>
@@ -63681,7 +63677,7 @@
         <v>2069.1669999999999</v>
       </c>
     </row>
-    <row r="2730" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2730" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2730" s="1">
         <v>44750</v>
       </c>
@@ -63704,7 +63700,7 @@
         <v>1526.5</v>
       </c>
     </row>
-    <row r="2731" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2731" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2731" s="1">
         <v>44750</v>
       </c>
@@ -63727,7 +63723,7 @@
         <v>1652.5</v>
       </c>
     </row>
-    <row r="2732" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2732" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2732" s="1">
         <v>44750</v>
       </c>
@@ -63750,7 +63746,7 @@
         <v>1794.5</v>
       </c>
     </row>
-    <row r="2733" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2733" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2733" s="1">
         <v>44750</v>
       </c>
@@ -63773,7 +63769,7 @@
         <v>2088.5</v>
       </c>
     </row>
-    <row r="2734" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2734" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2734" s="1">
         <v>44750</v>
       </c>
@@ -63796,7 +63792,7 @@
         <v>1760.5</v>
       </c>
     </row>
-    <row r="2735" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2735" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2735" s="1">
         <v>44750</v>
       </c>
@@ -63819,7 +63815,7 @@
         <v>1884.5</v>
       </c>
     </row>
-    <row r="2736" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2736" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2736" s="1">
         <v>44750</v>
       </c>
@@ -63842,7 +63838,7 @@
         <v>1992.5</v>
       </c>
     </row>
-    <row r="2737" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2737" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2737" s="1">
         <v>44750</v>
       </c>
@@ -63865,7 +63861,7 @@
         <v>2148.5</v>
       </c>
     </row>
-    <row r="2738" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2738" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2738" s="1">
         <v>44750</v>
       </c>
@@ -63888,7 +63884,7 @@
         <v>1838.1669999999999</v>
       </c>
     </row>
-    <row r="2739" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2739" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2739" s="1">
         <v>44750</v>
       </c>
@@ -63911,7 +63907,7 @@
         <v>1952.8330000000001</v>
       </c>
     </row>
-    <row r="2740" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2740" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2740" s="1">
         <v>44750</v>
       </c>
@@ -63934,7 +63930,7 @@
         <v>2014.1669999999999</v>
       </c>
     </row>
-    <row r="2741" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2741" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2741" s="1">
         <v>44750</v>
       </c>
@@ -63957,7 +63953,7 @@
         <v>2143.5</v>
       </c>
     </row>
-    <row r="2742" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2742" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2742" s="1">
         <v>44750</v>
       </c>
@@ -63980,7 +63976,7 @@
         <v>1544.5</v>
       </c>
     </row>
-    <row r="2743" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2743" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2743" s="1">
         <v>44750</v>
       </c>
@@ -64003,7 +63999,7 @@
         <v>1748.5</v>
       </c>
     </row>
-    <row r="2744" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2744" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2744" s="1">
         <v>44750</v>
       </c>
@@ -64026,7 +64022,7 @@
         <v>1898.5</v>
       </c>
     </row>
-    <row r="2745" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2745" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2745" s="1">
         <v>44750</v>
       </c>
@@ -64049,7 +64045,7 @@
         <v>2188.5</v>
       </c>
     </row>
-    <row r="2746" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2746" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2746" s="1">
         <v>44750</v>
       </c>
@@ -64072,7 +64068,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="2747" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2747" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2747" s="1">
         <v>44750</v>
       </c>
@@ -64095,7 +64091,7 @@
         <v>1719.8330000000001</v>
       </c>
     </row>
-    <row r="2748" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2748" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2748" s="1">
         <v>44750</v>
       </c>
@@ -64118,7 +64114,7 @@
         <v>1883.8330000000001</v>
       </c>
     </row>
-    <row r="2749" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2749" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2749" s="1">
         <v>44750</v>
       </c>
@@ -64141,7 +64137,7 @@
         <v>2077.1669999999999</v>
       </c>
     </row>
-    <row r="2750" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2750" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2750" s="1">
         <v>44750</v>
       </c>
@@ -64164,7 +64160,7 @@
         <v>1557.5</v>
       </c>
     </row>
-    <row r="2751" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2751" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2751" s="1">
         <v>44750</v>
       </c>
@@ -64187,7 +64183,7 @@
         <v>1685.5</v>
       </c>
     </row>
-    <row r="2752" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2752" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2752" s="1">
         <v>44750</v>
       </c>
@@ -64210,7 +64206,7 @@
         <v>1877.5</v>
       </c>
     </row>
-    <row r="2753" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2753" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2753" s="1">
         <v>44750</v>
       </c>
@@ -64233,7 +64229,7 @@
         <v>2125.5</v>
       </c>
     </row>
-    <row r="2754" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2754" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2754" s="1">
         <v>44750</v>
       </c>
@@ -64256,7 +64252,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="2755" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2755" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2755" s="1">
         <v>44750</v>
       </c>
@@ -64279,7 +64275,7 @@
         <v>1861.5</v>
       </c>
     </row>
-    <row r="2756" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2756" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2756" s="1">
         <v>44750</v>
       </c>
@@ -64302,7 +64298,7 @@
         <v>2007.5</v>
       </c>
     </row>
-    <row r="2757" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2757" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2757" s="1">
         <v>44750</v>
       </c>
@@ -64325,7 +64321,7 @@
         <v>2171.5</v>
       </c>
     </row>
-    <row r="2758" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2758" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2758" s="1">
         <v>44750</v>
       </c>
@@ -64348,7 +64344,7 @@
         <v>2053.5</v>
       </c>
     </row>
-    <row r="2759" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2759" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2759" s="1">
         <v>44750</v>
       </c>
@@ -64371,7 +64367,7 @@
         <v>2119.5</v>
       </c>
     </row>
-    <row r="2760" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2760" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2760" s="1">
         <v>44750</v>
       </c>
@@ -64394,7 +64390,7 @@
         <v>2197.5</v>
       </c>
     </row>
-    <row r="2761" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2761" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2761" s="1">
         <v>44750</v>
       </c>
@@ -64417,7 +64413,7 @@
         <v>2295.5</v>
       </c>
     </row>
-    <row r="2762" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2762" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2762" s="1">
         <v>44750</v>
       </c>
@@ -64440,7 +64436,7 @@
         <v>1827.8330000000001</v>
       </c>
     </row>
-    <row r="2763" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2763" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2763" s="1">
         <v>44750</v>
       </c>
@@ -64463,7 +64459,7 @@
         <v>1923.8330000000001</v>
       </c>
     </row>
-    <row r="2764" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2764" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2764" s="1">
         <v>44750</v>
       </c>
@@ -64486,7 +64482,7 @@
         <v>2077.1669999999999</v>
       </c>
     </row>
-    <row r="2765" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2765" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2765" s="1">
         <v>44750</v>
       </c>
@@ -64509,7 +64505,7 @@
         <v>2250.5</v>
       </c>
     </row>
-    <row r="2766" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2766" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2766" s="1">
         <v>44750</v>
       </c>
@@ -64532,7 +64528,7 @@
         <v>2086.5</v>
       </c>
     </row>
-    <row r="2767" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2767" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2767" s="1">
         <v>44750</v>
       </c>
@@ -64555,7 +64551,7 @@
         <v>2150.5</v>
       </c>
     </row>
-    <row r="2768" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2768" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2768" s="1">
         <v>44750</v>
       </c>
@@ -64578,7 +64574,7 @@
         <v>2193.1669999999999</v>
       </c>
     </row>
-    <row r="2769" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2769" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2769" s="1">
         <v>44750</v>
       </c>
@@ -64601,7 +64597,7 @@
         <v>2266.5</v>
       </c>
     </row>
-    <row r="2770" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2770" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2770" s="1">
         <v>44750</v>
       </c>
@@ -64624,7 +64620,7 @@
         <v>1780.5</v>
       </c>
     </row>
-    <row r="2771" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2771" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2771" s="1">
         <v>44750</v>
       </c>
@@ -64647,7 +64643,7 @@
         <v>1902.5</v>
       </c>
     </row>
-    <row r="2772" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2772" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2772" s="1">
         <v>44750</v>
       </c>
@@ -64670,7 +64666,7 @@
         <v>2012.5</v>
       </c>
     </row>
-    <row r="2773" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2773" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2773" s="1">
         <v>44750</v>
       </c>
@@ -64693,7 +64689,7 @@
         <v>2190.5</v>
       </c>
     </row>
-    <row r="2774" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2774" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2774" s="1">
         <v>44750</v>
       </c>
@@ -64716,7 +64712,7 @@
         <v>2250.5</v>
       </c>
     </row>
-    <row r="2775" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2775" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2775" s="1">
         <v>44750</v>
       </c>
@@ -64739,7 +64735,7 @@
         <v>2288.5</v>
       </c>
     </row>
-    <row r="2776" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2776" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2776" s="1">
         <v>44750</v>
       </c>
@@ -64762,7 +64758,7 @@
         <v>2246.5</v>
       </c>
     </row>
-    <row r="2777" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2777" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2777" s="1">
         <v>44750</v>
       </c>
@@ -64785,7 +64781,7 @@
         <v>2292.5</v>
       </c>
     </row>
-    <row r="2778" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2778" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2778" s="1">
         <v>44750</v>
       </c>
@@ -64808,7 +64804,7 @@
         <v>2229.5</v>
       </c>
     </row>
-    <row r="2779" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2779" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2779" s="1">
         <v>44750</v>
       </c>
@@ -64831,7 +64827,7 @@
         <v>2225.5</v>
       </c>
     </row>
-    <row r="2780" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2780" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2780" s="1">
         <v>44750</v>
       </c>
@@ -64854,7 +64850,7 @@
         <v>2182.5</v>
       </c>
     </row>
-    <row r="2781" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2781" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2781" s="1">
         <v>44750</v>
       </c>
@@ -64877,7 +64873,7 @@
         <v>2201.5</v>
       </c>
     </row>
-    <row r="2782" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2782" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2782" s="1">
         <v>44750</v>
       </c>
@@ -64900,7 +64896,7 @@
         <v>1530.5</v>
       </c>
     </row>
-    <row r="2783" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2783" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2783" s="1">
         <v>44750</v>
       </c>
@@ -64923,7 +64919,7 @@
         <v>1618.5</v>
       </c>
     </row>
-    <row r="2784" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2784" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2784" s="1">
         <v>44750</v>
       </c>
@@ -64946,7 +64942,7 @@
         <v>1744.5</v>
       </c>
     </row>
-    <row r="2785" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2785" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2785" s="1">
         <v>44750</v>
       </c>
@@ -64969,7 +64965,7 @@
         <v>2022.5</v>
       </c>
     </row>
-    <row r="2786" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2786" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2786" s="1">
         <v>44750</v>
       </c>
@@ -64992,7 +64988,7 @@
         <v>1674.5</v>
       </c>
     </row>
-    <row r="2787" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2787" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2787" s="1">
         <v>44750</v>
       </c>
@@ -65015,7 +65011,7 @@
         <v>1810.5</v>
       </c>
     </row>
-    <row r="2788" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2788" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2788" s="1">
         <v>44750</v>
       </c>
@@ -65038,7 +65034,7 @@
         <v>2078.5</v>
       </c>
     </row>
-    <row r="2789" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2789" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2789" s="1">
         <v>44750</v>
       </c>
@@ -65061,7 +65057,7 @@
         <v>2166.5</v>
       </c>
     </row>
-    <row r="2790" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2790" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2790" s="1">
         <v>44750</v>
       </c>
@@ -65084,7 +65080,7 @@
         <v>1952.5</v>
       </c>
     </row>
-    <row r="2791" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2791" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2791" s="1">
         <v>44750</v>
       </c>
@@ -65107,7 +65103,7 @@
         <v>2072.5</v>
       </c>
     </row>
-    <row r="2792" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2792" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2792" s="1">
         <v>44750</v>
       </c>
@@ -65130,7 +65126,7 @@
         <v>2141.8330000000001</v>
       </c>
     </row>
-    <row r="2793" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2793" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2793" s="1">
         <v>44750</v>
       </c>
@@ -65153,7 +65149,7 @@
         <v>2227.1669999999999</v>
       </c>
     </row>
-    <row r="2794" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2794" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2794" s="1">
         <v>44750</v>
       </c>
@@ -65176,7 +65172,7 @@
         <v>1873.8330000000001</v>
       </c>
     </row>
-    <row r="2795" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2795" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2795" s="1">
         <v>44750</v>
       </c>
@@ -65199,7 +65195,7 @@
         <v>1996.5</v>
       </c>
     </row>
-    <row r="2796" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2796" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2796" s="1">
         <v>44750</v>
       </c>
@@ -65222,7 +65218,7 @@
         <v>2084.5</v>
       </c>
     </row>
-    <row r="2797" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2797" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2797" s="1">
         <v>44750</v>
       </c>
@@ -65245,7 +65241,7 @@
         <v>2207.1669999999999</v>
       </c>
     </row>
-    <row r="2798" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2798" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2798" s="1">
         <v>44750</v>
       </c>
@@ -65268,7 +65264,7 @@
         <v>1763.1669999999999</v>
       </c>
     </row>
-    <row r="2799" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2799" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2799" s="1">
         <v>44750</v>
       </c>
@@ -65291,7 +65287,7 @@
         <v>1904.5</v>
       </c>
     </row>
-    <row r="2800" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2800" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2800" s="1">
         <v>44750</v>
       </c>
@@ -65314,7 +65310,7 @@
         <v>1983.1669999999999</v>
       </c>
     </row>
-    <row r="2801" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2801" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2801" s="1">
         <v>44750</v>
       </c>
@@ -65337,7 +65333,7 @@
         <v>2185.8330000000001</v>
       </c>
     </row>
-    <row r="2802" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2802" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2802" s="1">
         <v>44750</v>
       </c>
@@ -65360,7 +65356,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="2803" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2803" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2803" s="1">
         <v>44750</v>
       </c>
@@ -65383,7 +65379,7 @@
         <v>2229.5</v>
       </c>
     </row>
-    <row r="2804" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2804" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2804" s="1">
         <v>44750</v>
       </c>
@@ -65406,7 +65402,7 @@
         <v>2176.5</v>
       </c>
     </row>
-    <row r="2805" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2805" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2805" s="1">
         <v>44750</v>
       </c>
@@ -65429,7 +65425,7 @@
         <v>2236.5</v>
       </c>
     </row>
-    <row r="2806" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2806" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2806" s="1">
         <v>44750</v>
       </c>
@@ -65452,7 +65448,7 @@
         <v>2093.5</v>
       </c>
     </row>
-    <row r="2807" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2807" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2807" s="1">
         <v>44750</v>
       </c>
@@ -65475,7 +65471,7 @@
         <v>2097.5</v>
       </c>
     </row>
-    <row r="2808" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2808" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2808" s="1">
         <v>44750</v>
       </c>
@@ -65498,7 +65494,7 @@
         <v>2178.8330000000001</v>
       </c>
     </row>
-    <row r="2809" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2809" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2809" s="1">
         <v>44750</v>
       </c>
@@ -65521,7 +65517,7 @@
         <v>2085.5</v>
       </c>
     </row>
-    <row r="2810" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2810" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2810" s="1">
         <v>44750</v>
       </c>
@@ -65544,7 +65540,7 @@
         <v>2140.5</v>
       </c>
     </row>
-    <row r="2811" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2811" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2811" s="1">
         <v>44750</v>
       </c>
@@ -65567,7 +65563,7 @@
         <v>2155.5</v>
       </c>
     </row>
-    <row r="2812" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2812" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2812" s="1">
         <v>44750</v>
       </c>
@@ -65590,7 +65586,7 @@
         <v>2112.5</v>
       </c>
     </row>
-    <row r="2813" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2813" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2813" s="1">
         <v>44750</v>
       </c>
@@ -65613,7 +65609,7 @@
         <v>2209.5</v>
       </c>
     </row>
-    <row r="2814" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2814" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2814" s="1">
         <v>44750</v>
       </c>
@@ -65636,7 +65632,7 @@
         <v>2138.5</v>
       </c>
     </row>
-    <row r="2815" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2815" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2815" s="1">
         <v>44750</v>
       </c>
@@ -65659,7 +65655,7 @@
         <v>2130.5</v>
       </c>
     </row>
-    <row r="2816" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2816" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2816" s="1">
         <v>44750</v>
       </c>
@@ -65682,7 +65678,7 @@
         <v>2172.5</v>
       </c>
     </row>
-    <row r="2817" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2817" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2817" s="1">
         <v>44750</v>
       </c>
@@ -65705,7 +65701,7 @@
         <v>2220.5</v>
       </c>
     </row>
-    <row r="2818" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2818" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2818" s="1">
         <v>44750</v>
       </c>
@@ -65728,7 +65724,7 @@
         <v>2195.5</v>
       </c>
     </row>
-    <row r="2819" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2819" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2819" s="1">
         <v>44750</v>
       </c>
@@ -65751,7 +65747,7 @@
         <v>2238.5</v>
       </c>
     </row>
-    <row r="2820" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2820" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2820" s="1">
         <v>44750</v>
       </c>
@@ -65774,7 +65770,7 @@
         <v>2205.5</v>
       </c>
     </row>
-    <row r="2821" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2821" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2821" s="1">
         <v>44750</v>
       </c>
@@ -65797,7 +65793,7 @@
         <v>2242.5</v>
       </c>
     </row>
-    <row r="2822" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2822" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2822" s="1">
         <v>44750</v>
       </c>
@@ -65820,7 +65816,7 @@
         <v>2132.5</v>
       </c>
     </row>
-    <row r="2823" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2823" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2823" s="1">
         <v>44750</v>
       </c>
@@ -65843,7 +65839,7 @@
         <v>2207.5</v>
       </c>
     </row>
-    <row r="2824" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2824" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2824" s="1">
         <v>44750</v>
       </c>
@@ -65866,7 +65862,7 @@
         <v>2120.5</v>
       </c>
     </row>
-    <row r="2825" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2825" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2825" s="1">
         <v>44750</v>
       </c>
@@ -65889,7 +65885,7 @@
         <v>2233.5</v>
       </c>
     </row>
-    <row r="2826" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2826" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2826" s="1">
         <v>44750</v>
       </c>
@@ -65912,7 +65908,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="2827" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2827" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2827" s="1">
         <v>44750</v>
       </c>
@@ -65935,7 +65931,7 @@
         <v>2091.5</v>
       </c>
     </row>
-    <row r="2828" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2828" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2828" s="1">
         <v>44750</v>
       </c>
@@ -65958,7 +65954,7 @@
         <v>2121.5</v>
       </c>
     </row>
-    <row r="2829" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2829" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2829" s="1">
         <v>44750</v>
       </c>
@@ -65981,7 +65977,7 @@
         <v>2129.5</v>
       </c>
     </row>
-    <row r="2830" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2830" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2830" s="1">
         <v>44750</v>
       </c>
@@ -66004,7 +66000,7 @@
         <v>2159.5</v>
       </c>
     </row>
-    <row r="2831" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2831" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2831" s="1">
         <v>44750</v>
       </c>
@@ -66027,7 +66023,7 @@
         <v>2147.5</v>
       </c>
     </row>
-    <row r="2832" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2832" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2832" s="1">
         <v>44750</v>
       </c>
@@ -66050,7 +66046,7 @@
         <v>2113.5</v>
       </c>
     </row>
-    <row r="2833" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2833" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2833" s="1">
         <v>44750</v>
       </c>
@@ -66073,7 +66069,7 @@
         <v>2103.5</v>
       </c>
     </row>
-    <row r="2834" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2834" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2834" s="1">
         <v>44750</v>
       </c>
@@ -66096,7 +66092,7 @@
         <v>2004.5</v>
       </c>
     </row>
-    <row r="2835" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2835" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2835" s="1">
         <v>44750</v>
       </c>
@@ -66119,7 +66115,7 @@
         <v>2040.5</v>
       </c>
     </row>
-    <row r="2836" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2836" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2836" s="1">
         <v>44750</v>
       </c>
@@ -66142,7 +66138,7 @@
         <v>2100.5</v>
       </c>
     </row>
-    <row r="2837" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2837" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2837" s="1">
         <v>44750</v>
       </c>
@@ -66165,7 +66161,7 @@
         <v>2110.5</v>
       </c>
     </row>
-    <row r="2838" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2838" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2838" s="1">
         <v>44750</v>
       </c>
@@ -66188,7 +66184,7 @@
         <v>2082.5</v>
       </c>
     </row>
-    <row r="2839" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2839" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2839" s="1">
         <v>44750</v>
       </c>
@@ -66211,7 +66207,7 @@
         <v>2084.5</v>
       </c>
     </row>
-    <row r="2840" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2840" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2840" s="1">
         <v>44750</v>
       </c>
@@ -66234,7 +66230,7 @@
         <v>2118.5</v>
       </c>
     </row>
-    <row r="2841" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2841" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2841" s="1">
         <v>44750</v>
       </c>
@@ -66257,7 +66253,7 @@
         <v>2138.5</v>
       </c>
     </row>
-    <row r="2842" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2842" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2842" s="1">
         <v>44750</v>
       </c>
@@ -66280,7 +66276,7 @@
         <v>2102.5</v>
       </c>
     </row>
-    <row r="2843" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2843" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2843" s="1">
         <v>44750</v>
       </c>
@@ -66303,7 +66299,7 @@
         <v>2088.5</v>
       </c>
     </row>
-    <row r="2844" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2844" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2844" s="1">
         <v>44750</v>
       </c>
@@ -66326,7 +66322,7 @@
         <v>2084.5</v>
       </c>
     </row>
-    <row r="2845" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2845" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2845" s="1">
         <v>44750</v>
       </c>
@@ -66349,7 +66345,7 @@
         <v>2072.5</v>
       </c>
     </row>
-    <row r="2846" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2846" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2846" s="1">
         <v>44750</v>
       </c>
@@ -66372,7 +66368,7 @@
         <v>2088.5</v>
       </c>
     </row>
-    <row r="2847" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2847" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2847" s="1">
         <v>44750</v>
       </c>
@@ -66395,7 +66391,7 @@
         <v>2086.5</v>
       </c>
     </row>
-    <row r="2848" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2848" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2848" s="1">
         <v>44750</v>
       </c>
@@ -66418,7 +66414,7 @@
         <v>2098.5</v>
       </c>
     </row>
-    <row r="2849" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2849" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2849" s="1">
         <v>44750</v>
       </c>
@@ -66441,7 +66437,7 @@
         <v>2128.5</v>
       </c>
     </row>
-    <row r="2850" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2850" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2850" s="1">
         <v>44750</v>
       </c>
@@ -66464,7 +66460,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="2851" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2851" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2851" s="1">
         <v>44750</v>
       </c>
@@ -66487,7 +66483,7 @@
         <v>2152.5</v>
       </c>
     </row>
-    <row r="2852" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2852" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2852" s="1">
         <v>44750</v>
       </c>
@@ -66510,7 +66506,7 @@
         <v>2136.5</v>
       </c>
     </row>
-    <row r="2853" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2853" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2853" s="1">
         <v>44750</v>
       </c>
@@ -66533,7 +66529,7 @@
         <v>2128.5</v>
       </c>
     </row>
-    <row r="2854" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2854" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2854" s="1">
         <v>44750</v>
       </c>
@@ -66556,7 +66552,7 @@
         <v>2132.5</v>
       </c>
     </row>
-    <row r="2855" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2855" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2855" s="1">
         <v>44750</v>
       </c>
@@ -66579,7 +66575,7 @@
         <v>2102.5</v>
       </c>
     </row>
-    <row r="2856" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2856" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2856" s="1">
         <v>44750</v>
       </c>
@@ -66602,7 +66598,7 @@
         <v>2114.5</v>
       </c>
     </row>
-    <row r="2857" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2857" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2857" s="1">
         <v>44750</v>
       </c>
@@ -66625,7 +66621,7 @@
         <v>2134.5</v>
       </c>
     </row>
-    <row r="2858" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2858" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2858" s="1">
         <v>44750</v>
       </c>
@@ -66648,7 +66644,7 @@
         <v>2147.5</v>
       </c>
     </row>
-    <row r="2859" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2859" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2859" s="1">
         <v>44750</v>
       </c>
@@ -66671,7 +66667,7 @@
         <v>2119.5</v>
       </c>
     </row>
-    <row r="2860" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2860" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2860" s="1">
         <v>44750</v>
       </c>
@@ -66694,7 +66690,7 @@
         <v>2151.5</v>
       </c>
     </row>
-    <row r="2861" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2861" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2861" s="1">
         <v>44750</v>
       </c>
@@ -66717,7 +66713,7 @@
         <v>2155.5</v>
       </c>
     </row>
-    <row r="2862" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2862" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2862" s="1">
         <v>44750</v>
       </c>
@@ -66740,7 +66736,7 @@
         <v>2127.5</v>
       </c>
     </row>
-    <row r="2863" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2863" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2863" s="1">
         <v>44750</v>
       </c>
@@ -66763,7 +66759,7 @@
         <v>2071.5</v>
       </c>
     </row>
-    <row r="2864" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2864" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2864" s="1">
         <v>44750</v>
       </c>
@@ -66786,7 +66782,7 @@
         <v>2039.5</v>
       </c>
     </row>
-    <row r="2865" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2865" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2865" s="1">
         <v>44750</v>
       </c>
@@ -66809,7 +66805,7 @@
         <v>2071.5</v>
       </c>
     </row>
-    <row r="2866" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2866" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2866" s="1">
         <v>44750</v>
       </c>
@@ -66832,7 +66828,7 @@
         <v>2136.5</v>
       </c>
     </row>
-    <row r="2867" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2867" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2867" s="1">
         <v>44750</v>
       </c>
@@ -66855,7 +66851,7 @@
         <v>2137.8330000000001</v>
       </c>
     </row>
-    <row r="2868" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2868" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2868" s="1">
         <v>44750</v>
       </c>
@@ -66878,7 +66874,7 @@
         <v>2141.8330000000001</v>
       </c>
     </row>
-    <row r="2869" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2869" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2869" s="1">
         <v>44750</v>
       </c>
@@ -66901,7 +66897,7 @@
         <v>2188.5</v>
       </c>
     </row>
-    <row r="2870" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2870" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2870" s="1">
         <v>44750</v>
       </c>
@@ -66924,7 +66920,7 @@
         <v>2044.5</v>
       </c>
     </row>
-    <row r="2871" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2871" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2871" s="1">
         <v>44750</v>
       </c>
@@ -66947,7 +66943,7 @@
         <v>2064.5</v>
       </c>
     </row>
-    <row r="2872" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2872" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2872" s="1">
         <v>44750</v>
       </c>
@@ -66970,7 +66966,7 @@
         <v>2070.5</v>
       </c>
     </row>
-    <row r="2873" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2873" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2873" s="1">
         <v>44750</v>
       </c>
@@ -66993,7 +66989,7 @@
         <v>2100.5</v>
       </c>
     </row>
-    <row r="2874" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2874" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2874" s="1">
         <v>44750</v>
       </c>
@@ -67016,7 +67012,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="2875" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2875" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2875" s="1">
         <v>44750</v>
       </c>
@@ -67039,7 +67035,7 @@
         <v>2137.8330000000001</v>
       </c>
     </row>
-    <row r="2876" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2876" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2876" s="1">
         <v>44750</v>
       </c>
@@ -67062,7 +67058,7 @@
         <v>2139.1669999999999</v>
       </c>
     </row>
-    <row r="2877" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2877" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2877" s="1">
         <v>44750</v>
       </c>
@@ -67085,7 +67081,7 @@
         <v>2223.1669999999999</v>
       </c>
     </row>
-    <row r="2878" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2878" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2878" s="1">
         <v>44750</v>
       </c>
@@ -67108,7 +67104,7 @@
         <v>2114.5</v>
       </c>
     </row>
-    <row r="2879" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2879" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2879" s="1">
         <v>44750</v>
       </c>
@@ -67131,7 +67127,7 @@
         <v>2076.5</v>
       </c>
     </row>
-    <row r="2880" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2880" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2880" s="1">
         <v>44750</v>
       </c>
@@ -67154,7 +67150,7 @@
         <v>2072.5</v>
       </c>
     </row>
-    <row r="2881" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2881" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2881" s="1">
         <v>44750</v>
       </c>
@@ -67177,7 +67173,7 @@
         <v>2088.5</v>
       </c>
     </row>
-    <row r="2882" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2882" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2882" s="1">
         <v>44750</v>
       </c>
@@ -67200,7 +67196,7 @@
         <v>2108.5</v>
       </c>
     </row>
-    <row r="2883" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2883" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2883" s="1">
         <v>44750</v>
       </c>
@@ -67223,7 +67219,7 @@
         <v>2106.5</v>
       </c>
     </row>
-    <row r="2884" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2884" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2884" s="1">
         <v>44750</v>
       </c>
@@ -67246,7 +67242,7 @@
         <v>2086.5</v>
       </c>
     </row>
-    <row r="2885" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2885" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2885" s="1">
         <v>44750</v>
       </c>
@@ -67269,7 +67265,7 @@
         <v>2096.5</v>
       </c>
     </row>
-    <row r="2886" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2886" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2886" s="1">
         <v>44750</v>
       </c>
@@ -67292,7 +67288,7 @@
         <v>2180.5</v>
       </c>
     </row>
-    <row r="2887" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2887" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2887" s="1">
         <v>44750</v>
       </c>
@@ -67315,7 +67311,7 @@
         <v>2164.5</v>
       </c>
     </row>
-    <row r="2888" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2888" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2888" s="1">
         <v>44750</v>
       </c>
@@ -67338,7 +67334,7 @@
         <v>2170.5</v>
       </c>
     </row>
-    <row r="2889" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2889" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2889" s="1">
         <v>44750</v>
       </c>
@@ -67361,7 +67357,7 @@
         <v>2182.5</v>
       </c>
     </row>
-    <row r="2890" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2890" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2890" s="1">
         <v>44750</v>
       </c>
@@ -67384,7 +67380,7 @@
         <v>2172.5</v>
       </c>
     </row>
-    <row r="2891" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2891" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2891" s="1">
         <v>44750</v>
       </c>
@@ -67407,7 +67403,7 @@
         <v>2176.5</v>
       </c>
     </row>
-    <row r="2892" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2892" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2892" s="1">
         <v>44750</v>
       </c>
@@ -67430,7 +67426,7 @@
         <v>2192.5</v>
       </c>
     </row>
-    <row r="2893" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2893" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2893" s="1">
         <v>44750</v>
       </c>
@@ -67453,7 +67449,7 @@
         <v>2206.5</v>
       </c>
     </row>
-    <row r="2894" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2894" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2894" s="1">
         <v>44750</v>
       </c>
@@ -67476,7 +67472,7 @@
         <v>2153.8330000000001</v>
       </c>
     </row>
-    <row r="2895" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2895" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2895" s="1">
         <v>44750</v>
       </c>
@@ -67499,7 +67495,7 @@
         <v>2136.5</v>
       </c>
     </row>
-    <row r="2896" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2896" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2896" s="1">
         <v>44750</v>
       </c>
@@ -67522,7 +67518,7 @@
         <v>2135.1669999999999</v>
       </c>
     </row>
-    <row r="2897" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2897" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2897" s="1">
         <v>44750</v>
       </c>
@@ -67545,7 +67541,7 @@
         <v>2209.8330000000001</v>
       </c>
     </row>
-    <row r="2898" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2898" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2898" s="1">
         <v>44750</v>
       </c>
@@ -67568,7 +67564,7 @@
         <v>2064</v>
       </c>
     </row>
-    <row r="2899" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2899" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2899" s="1">
         <v>44750</v>
       </c>
@@ -67591,7 +67587,7 @@
         <v>2021.1669999999999</v>
       </c>
     </row>
-    <row r="2900" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2900" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2900" s="1">
         <v>44750</v>
       </c>
@@ -67614,7 +67610,7 @@
         <v>2046.5</v>
       </c>
     </row>
-    <row r="2901" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2901" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2901" s="1">
         <v>44750</v>
       </c>
@@ -67637,7 +67633,7 @@
         <v>2021.1669999999999</v>
       </c>
     </row>
-    <row r="2902" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2902" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2902" s="1">
         <v>44750</v>
       </c>
@@ -67660,7 +67656,7 @@
         <v>2080.8330000000001</v>
       </c>
     </row>
-    <row r="2903" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2903" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2903" s="1">
         <v>44750</v>
       </c>
@@ -67683,7 +67679,7 @@
         <v>2044.8330000000001</v>
       </c>
     </row>
-    <row r="2904" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2904" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2904" s="1">
         <v>44750</v>
       </c>
@@ -67706,7 +67702,7 @@
         <v>2032.8330000000001</v>
       </c>
     </row>
-    <row r="2905" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2905" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2905" s="1">
         <v>44750</v>
       </c>
@@ -67729,7 +67725,7 @@
         <v>2031.5</v>
       </c>
     </row>
-    <row r="2906" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2906" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2906" s="1">
         <v>44750</v>
       </c>
@@ -67752,7 +67748,7 @@
         <v>2057.1669999999999</v>
       </c>
     </row>
-    <row r="2907" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2907" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2907" s="1">
         <v>44750</v>
       </c>
@@ -67775,7 +67771,7 @@
         <v>2055.8330000000001</v>
       </c>
     </row>
-    <row r="2908" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2908" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2908" s="1">
         <v>44750</v>
       </c>
@@ -67798,7 +67794,7 @@
         <v>2067.8330000000001</v>
       </c>
     </row>
-    <row r="2909" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2909" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2909" s="1">
         <v>44750</v>
       </c>
@@ -67821,7 +67817,7 @@
         <v>2094.5</v>
       </c>
     </row>
-    <row r="2910" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2910" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2910" s="1">
         <v>44750</v>
       </c>
@@ -67844,7 +67840,7 @@
         <v>2145.1669999999999</v>
       </c>
     </row>
-    <row r="2911" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2911" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2911" s="1">
         <v>44750</v>
       </c>
@@ -67867,7 +67863,7 @@
         <v>2097.1669999999999</v>
       </c>
     </row>
-    <row r="2912" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2912" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2912" s="1">
         <v>44750</v>
       </c>
@@ -67890,7 +67886,7 @@
         <v>2095.8330000000001</v>
       </c>
     </row>
-    <row r="2913" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2913" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2913" s="1">
         <v>44750</v>
       </c>
@@ -67913,7 +67909,7 @@
         <v>2101.1669999999999</v>
       </c>
     </row>
-    <row r="2914" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2914" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2914" s="1">
         <v>44750</v>
       </c>
@@ -67936,7 +67932,7 @@
         <v>2082.5</v>
       </c>
     </row>
-    <row r="2915" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2915" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2915" s="1">
         <v>44750</v>
       </c>
@@ -67959,7 +67955,7 @@
         <v>2054.5</v>
       </c>
     </row>
-    <row r="2916" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2916" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2916" s="1">
         <v>44750</v>
       </c>
@@ -67982,7 +67978,7 @@
         <v>2054.5</v>
       </c>
     </row>
-    <row r="2917" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2917" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2917" s="1">
         <v>44750</v>
       </c>
@@ -68005,7 +68001,7 @@
         <v>2062.5</v>
       </c>
     </row>
-    <row r="2918" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2918" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2918" s="1">
         <v>44750</v>
       </c>
@@ -68028,7 +68024,7 @@
         <v>2162.1669999999999</v>
       </c>
     </row>
-    <row r="2919" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2919" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2919" s="1">
         <v>44750</v>
       </c>
@@ -68051,7 +68047,7 @@
         <v>2106.1669999999999</v>
       </c>
     </row>
-    <row r="2920" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2920" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2920" s="1">
         <v>44750</v>
       </c>
@@ -68074,7 +68070,7 @@
         <v>2063.5</v>
       </c>
     </row>
-    <row r="2921" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2921" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2921" s="1">
         <v>44750</v>
       </c>
@@ -68097,7 +68093,7 @@
         <v>2058.1669999999999</v>
       </c>
     </row>
-    <row r="2922" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2922" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2922" s="1">
         <v>44750</v>
       </c>
@@ -68120,7 +68116,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="2923" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2923" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2923" s="1">
         <v>44750</v>
       </c>
@@ -68143,7 +68139,7 @@
         <v>2179.5</v>
       </c>
     </row>
-    <row r="2924" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2924" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2924" s="1">
         <v>44750</v>
       </c>
@@ -68166,7 +68162,7 @@
         <v>2162.5</v>
       </c>
     </row>
-    <row r="2925" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2925" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2925" s="1">
         <v>44750</v>
       </c>
@@ -68189,7 +68185,7 @@
         <v>2165.5</v>
       </c>
     </row>
-    <row r="2926" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2926" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2926" s="1">
         <v>44750</v>
       </c>
@@ -68212,7 +68208,7 @@
         <v>2114.5</v>
       </c>
     </row>
-    <row r="2927" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2927" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2927" s="1">
         <v>44750</v>
       </c>
@@ -68235,7 +68231,7 @@
         <v>2093.1669999999999</v>
       </c>
     </row>
-    <row r="2928" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2928" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2928" s="1">
         <v>44750</v>
       </c>
@@ -68258,7 +68254,7 @@
         <v>2134.5</v>
       </c>
     </row>
-    <row r="2929" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2929" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2929" s="1">
         <v>44750</v>
       </c>
@@ -68281,7 +68277,7 @@
         <v>2126.5</v>
       </c>
     </row>
-    <row r="2930" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2930" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2930" s="1">
         <v>44750</v>
       </c>
@@ -68304,7 +68300,7 @@
         <v>2030.5</v>
       </c>
     </row>
-    <row r="2931" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2931" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2931" s="1">
         <v>44750</v>
       </c>
@@ -68327,7 +68323,7 @@
         <v>2041.1669999999999</v>
       </c>
     </row>
-    <row r="2932" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2932" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2932" s="1">
         <v>44750</v>
       </c>
@@ -68350,7 +68346,7 @@
         <v>2077.1669999999999</v>
       </c>
     </row>
-    <row r="2933" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2933" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2933" s="1">
         <v>44750</v>
       </c>
@@ -68373,7 +68369,7 @@
         <v>2167.8330000000001</v>
       </c>
     </row>
-    <row r="2934" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2934" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2934" s="1">
         <v>44750</v>
       </c>
@@ -68396,7 +68392,7 @@
         <v>2060.1669999999999</v>
       </c>
     </row>
-    <row r="2935" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2935" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2935" s="1">
         <v>44750</v>
       </c>
@@ -68419,7 +68415,7 @@
         <v>2084.1669999999999</v>
       </c>
     </row>
-    <row r="2936" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2936" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2936" s="1">
         <v>44750</v>
       </c>
@@ -68442,7 +68438,7 @@
         <v>2126.8330000000001</v>
       </c>
     </row>
-    <row r="2937" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2937" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2937" s="1">
         <v>44750</v>
       </c>
@@ -68465,7 +68461,7 @@
         <v>2181.5</v>
       </c>
     </row>
-    <row r="2938" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2938" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2938" s="1">
         <v>44750</v>
       </c>
@@ -68488,7 +68484,7 @@
         <v>2146.5</v>
       </c>
     </row>
-    <row r="2939" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2939" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2939" s="1">
         <v>44750</v>
       </c>
@@ -68511,7 +68507,7 @@
         <v>2071.8330000000001</v>
       </c>
     </row>
-    <row r="2940" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2940" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2940" s="1">
         <v>44750</v>
       </c>
@@ -68534,7 +68530,7 @@
         <v>2198.5</v>
       </c>
     </row>
-    <row r="2941" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2941" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2941" s="1">
         <v>44750</v>
       </c>
@@ -68557,7 +68553,7 @@
         <v>2161.1669999999999</v>
       </c>
     </row>
-    <row r="2942" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2942" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2942" s="1">
         <v>44750</v>
       </c>
@@ -68580,7 +68576,7 @@
         <v>2096.5</v>
       </c>
     </row>
-    <row r="2943" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2943" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2943" s="1">
         <v>44750</v>
       </c>
@@ -68603,7 +68599,7 @@
         <v>2133.8330000000001</v>
       </c>
     </row>
-    <row r="2944" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2944" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2944" s="1">
         <v>44750</v>
       </c>
@@ -68626,7 +68622,7 @@
         <v>2155.1669999999999</v>
       </c>
     </row>
-    <row r="2945" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2945" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2945" s="1">
         <v>44750</v>
       </c>
@@ -68649,7 +68645,7 @@
         <v>2193.8330000000001</v>
       </c>
     </row>
-    <row r="2946" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2946" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2946" s="1">
         <v>44750</v>
       </c>
@@ -68672,7 +68668,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="2947" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2947" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2947" s="1">
         <v>44750</v>
       </c>
@@ -68695,7 +68691,7 @@
         <v>2085.8330000000001</v>
       </c>
     </row>
-    <row r="2948" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2948" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2948" s="1">
         <v>44750</v>
       </c>
@@ -68718,7 +68714,7 @@
         <v>2068.5</v>
       </c>
     </row>
-    <row r="2949" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2949" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2949" s="1">
         <v>44750</v>
       </c>
@@ -68741,7 +68737,7 @@
         <v>2068.5</v>
       </c>
     </row>
-    <row r="2950" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2950" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2950" s="1">
         <v>44750</v>
       </c>
@@ -68764,7 +68760,7 @@
         <v>2076.8330000000001</v>
       </c>
     </row>
-    <row r="2951" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2951" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2951" s="1">
         <v>44750</v>
       </c>
@@ -68787,7 +68783,7 @@
         <v>2084.8330000000001</v>
       </c>
     </row>
-    <row r="2952" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2952" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2952" s="1">
         <v>44750</v>
       </c>
@@ -68810,7 +68806,7 @@
         <v>2115.5</v>
       </c>
     </row>
-    <row r="2953" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2953" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2953" s="1">
         <v>44750</v>
       </c>
@@ -68833,7 +68829,7 @@
         <v>2136.8330000000001</v>
       </c>
     </row>
-    <row r="2954" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2954" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2954" s="1">
         <v>44750</v>
       </c>
@@ -68856,7 +68852,7 @@
         <v>2013.8330000000001</v>
       </c>
     </row>
-    <row r="2955" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2955" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2955" s="1">
         <v>44750</v>
       </c>
@@ -68879,7 +68875,7 @@
         <v>2013.8330000000001</v>
       </c>
     </row>
-    <row r="2956" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2956" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2956" s="1">
         <v>44750</v>
       </c>
@@ -68902,7 +68898,7 @@
         <v>2095.1669999999999</v>
       </c>
     </row>
-    <row r="2957" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2957" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2957" s="1">
         <v>44750</v>
       </c>
@@ -68925,7 +68921,7 @@
         <v>2135.1669999999999</v>
       </c>
     </row>
-    <row r="2958" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2958" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2958" s="1">
         <v>44750</v>
       </c>
@@ -68948,7 +68944,7 @@
         <v>2166.8330000000001</v>
       </c>
     </row>
-    <row r="2959" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2959" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2959" s="1">
         <v>44750</v>
       </c>
@@ -68971,7 +68967,7 @@
         <v>2128.1669999999999</v>
       </c>
     </row>
-    <row r="2960" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2960" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2960" s="1">
         <v>44750</v>
       </c>
@@ -68994,7 +68990,7 @@
         <v>2145.5</v>
       </c>
     </row>
-    <row r="2961" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2961" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2961" s="1">
         <v>44750</v>
       </c>
@@ -69017,7 +69013,7 @@
         <v>2161.5</v>
       </c>
     </row>
-    <row r="2962" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2962" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2962" s="1">
         <v>44750</v>
       </c>
@@ -69040,7 +69036,7 @@
         <v>2174.5</v>
       </c>
     </row>
-    <row r="2963" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2963" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2963" s="1">
         <v>44750</v>
       </c>
@@ -69063,7 +69059,7 @@
         <v>2119.8330000000001</v>
       </c>
     </row>
-    <row r="2964" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2964" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2964" s="1">
         <v>44750</v>
       </c>
@@ -69086,7 +69082,7 @@
         <v>2170.5</v>
       </c>
     </row>
-    <row r="2965" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2965" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2965" s="1">
         <v>44750</v>
       </c>
@@ -69109,7 +69105,7 @@
         <v>2170.5</v>
       </c>
     </row>
-    <row r="2966" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2966" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2966" s="1">
         <v>44750</v>
       </c>
@@ -69132,7 +69128,7 @@
         <v>2153.5</v>
       </c>
     </row>
-    <row r="2967" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2967" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2967" s="1">
         <v>44750</v>
       </c>
@@ -69155,7 +69151,7 @@
         <v>2094.8330000000001</v>
       </c>
     </row>
-    <row r="2968" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2968" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2968" s="1">
         <v>44750</v>
       </c>
@@ -69178,7 +69174,7 @@
         <v>2089.5</v>
       </c>
     </row>
-    <row r="2969" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2969" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2969" s="1">
         <v>44750</v>
       </c>
@@ -69201,7 +69197,7 @@
         <v>2090.8330000000001</v>
       </c>
     </row>
-    <row r="2970" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2970" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2970" s="1">
         <v>44750</v>
       </c>
@@ -69224,7 +69220,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="2971" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2971" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2971" s="1">
         <v>44750</v>
       </c>
@@ -69247,7 +69243,7 @@
         <v>2137.1669999999999</v>
       </c>
     </row>
-    <row r="2972" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2972" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2972" s="1">
         <v>44750</v>
       </c>
@@ -69270,7 +69266,7 @@
         <v>2103.8330000000001</v>
       </c>
     </row>
-    <row r="2973" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2973" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2973" s="1">
         <v>44750</v>
       </c>
@@ -69293,7 +69289,7 @@
         <v>2121.1669999999999</v>
       </c>
     </row>
-    <row r="2974" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2974" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2974" s="1">
         <v>44750</v>
       </c>
@@ -69316,7 +69312,7 @@
         <v>2105.1669999999999</v>
       </c>
     </row>
-    <row r="2975" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2975" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2975" s="1">
         <v>44750</v>
       </c>
@@ -69339,7 +69335,7 @@
         <v>2061.1669999999999</v>
       </c>
     </row>
-    <row r="2976" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2976" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2976" s="1">
         <v>44750</v>
       </c>
@@ -69362,7 +69358,7 @@
         <v>2069.1669999999999</v>
       </c>
     </row>
-    <row r="2977" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2977" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2977" s="1">
         <v>44750</v>
       </c>
@@ -69385,7 +69381,7 @@
         <v>2047.8330000000001</v>
       </c>
     </row>
-    <row r="2978" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2978" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2978" s="1">
         <v>44750</v>
       </c>
@@ -69408,7 +69404,7 @@
         <v>2121.5</v>
       </c>
     </row>
-    <row r="2979" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2979" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2979" s="1">
         <v>44750</v>
       </c>
@@ -69431,7 +69427,7 @@
         <v>2104.1669999999999</v>
       </c>
     </row>
-    <row r="2980" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2980" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2980" s="1">
         <v>44750</v>
       </c>
@@ -69454,7 +69450,7 @@
         <v>2101.5</v>
       </c>
     </row>
-    <row r="2981" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2981" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2981" s="1">
         <v>44750</v>
       </c>
@@ -69477,7 +69473,7 @@
         <v>2100.1669999999999</v>
       </c>
     </row>
-    <row r="2982" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2982" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2982" s="1">
         <v>44750</v>
       </c>
@@ -69500,7 +69496,7 @@
         <v>2093.8330000000001</v>
       </c>
     </row>
-    <row r="2983" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2983" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2983" s="1">
         <v>44750</v>
       </c>
@@ -69523,7 +69519,7 @@
         <v>2079.1669999999999</v>
       </c>
     </row>
-    <row r="2984" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2984" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2984" s="1">
         <v>44750</v>
       </c>
@@ -69546,7 +69542,7 @@
         <v>2073.8330000000001</v>
       </c>
     </row>
-    <row r="2985" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2985" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2985" s="1">
         <v>44750</v>
       </c>
@@ -69569,7 +69565,7 @@
         <v>2108.5</v>
       </c>
     </row>
-    <row r="2986" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2986" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2986" s="1">
         <v>44750</v>
       </c>
@@ -69592,7 +69588,7 @@
         <v>2159.8330000000001</v>
       </c>
     </row>
-    <row r="2987" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2987" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2987" s="1">
         <v>44750</v>
       </c>
@@ -69615,7 +69611,7 @@
         <v>2153.1669999999999</v>
       </c>
     </row>
-    <row r="2988" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2988" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2988" s="1">
         <v>44750</v>
       </c>
@@ -69638,7 +69634,7 @@
         <v>2150.5</v>
       </c>
     </row>
-    <row r="2989" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2989" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2989" s="1">
         <v>44750</v>
       </c>
@@ -69661,7 +69657,7 @@
         <v>2154.5</v>
       </c>
     </row>
-    <row r="2990" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2990" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2990" s="1">
         <v>44750</v>
       </c>
@@ -69684,7 +69680,7 @@
         <v>2160.1669999999999</v>
       </c>
     </row>
-    <row r="2991" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2991" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2991" s="1">
         <v>44750</v>
       </c>
@@ -69707,7 +69703,7 @@
         <v>2168.1669999999999</v>
       </c>
     </row>
-    <row r="2992" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2992" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2992" s="1">
         <v>44750</v>
       </c>
@@ -69730,7 +69726,7 @@
         <v>2170.8330000000001</v>
       </c>
     </row>
-    <row r="2993" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2993" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2993" s="1">
         <v>44750</v>
       </c>
@@ -69753,7 +69749,7 @@
         <v>2193.5</v>
       </c>
     </row>
-    <row r="2994" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2994" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2994" s="1">
         <v>44750</v>
       </c>
@@ -69776,7 +69772,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="2995" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2995" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2995" s="1">
         <v>44750</v>
       </c>
@@ -69799,7 +69795,7 @@
         <v>2012.5</v>
       </c>
     </row>
-    <row r="2996" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2996" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2996" s="1">
         <v>44750</v>
       </c>
@@ -69822,7 +69818,7 @@
         <v>2007.1669999999999</v>
       </c>
     </row>
-    <row r="2997" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2997" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2997" s="1">
         <v>44750</v>
       </c>
@@ -69845,7 +69841,7 @@
         <v>1995.1669999999999</v>
       </c>
     </row>
-    <row r="2998" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2998" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2998" s="1">
         <v>44750</v>
       </c>
@@ -69868,7 +69864,7 @@
         <v>2034.5</v>
       </c>
     </row>
-    <row r="2999" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2999" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2999" s="1">
         <v>44750</v>
       </c>
@@ -69891,7 +69887,7 @@
         <v>2020.5</v>
       </c>
     </row>
-    <row r="3000" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3000" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3000" s="1">
         <v>44750</v>
       </c>
@@ -69914,7 +69910,7 @@
         <v>2036.5</v>
       </c>
     </row>
-    <row r="3001" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3001" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3001" s="1">
         <v>44750</v>
       </c>
@@ -69937,7 +69933,7 @@
         <v>2060.5</v>
       </c>
     </row>
-    <row r="3002" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3002" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3002" s="1">
         <v>44750</v>
       </c>
@@ -69960,7 +69956,7 @@
         <v>2078.5</v>
       </c>
     </row>
-    <row r="3003" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3003" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3003" s="1">
         <v>44750</v>
       </c>
@@ -69983,7 +69979,7 @@
         <v>2052.5</v>
       </c>
     </row>
-    <row r="3004" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3004" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3004" s="1">
         <v>44750</v>
       </c>
@@ -70006,7 +70002,7 @@
         <v>2036.5</v>
       </c>
     </row>
-    <row r="3005" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3005" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3005" s="1">
         <v>44750</v>
       </c>
@@ -70029,7 +70025,7 @@
         <v>2054.5</v>
       </c>
     </row>
-    <row r="3006" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3006" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3006" s="1">
         <v>44750</v>
       </c>
@@ -70052,7 +70048,7 @@
         <v>2022.5</v>
       </c>
     </row>
-    <row r="3007" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3007" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3007" s="1">
         <v>44750</v>
       </c>
@@ -70075,7 +70071,7 @@
         <v>2020.5</v>
       </c>
     </row>
-    <row r="3008" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3008" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3008" s="1">
         <v>44750</v>
       </c>
@@ -70098,7 +70094,7 @@
         <v>2010.5</v>
       </c>
     </row>
-    <row r="3009" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3009" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3009" s="1">
         <v>44750</v>
       </c>
@@ -70121,7 +70117,7 @@
         <v>2032.5</v>
       </c>
     </row>
-    <row r="3010" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3010" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3010" s="1">
         <v>44750</v>
       </c>
@@ -70144,7 +70140,7 @@
         <v>2032.5</v>
       </c>
     </row>
-    <row r="3011" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3011" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3011" s="1">
         <v>44750</v>
       </c>
@@ -70167,7 +70163,7 @@
         <v>2024.5</v>
       </c>
     </row>
-    <row r="3012" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3012" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3012" s="1">
         <v>44750</v>
       </c>
@@ -70190,7 +70186,7 @@
         <v>2012.5</v>
       </c>
     </row>
-    <row r="3013" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3013" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3013" s="1">
         <v>44750</v>
       </c>
@@ -70213,7 +70209,7 @@
         <v>1990.5</v>
       </c>
     </row>
-    <row r="3014" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3014" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3014" s="1">
         <v>44750</v>
       </c>
@@ -70236,7 +70232,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="3015" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3015" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3015" s="1">
         <v>44750</v>
       </c>
@@ -70259,7 +70255,7 @@
         <v>2124.5</v>
       </c>
     </row>
-    <row r="3016" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3016" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3016" s="1">
         <v>44750</v>
       </c>
@@ -70282,7 +70278,7 @@
         <v>2132.5</v>
       </c>
     </row>
-    <row r="3017" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3017" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3017" s="1">
         <v>44750</v>
       </c>
@@ -70305,7 +70301,7 @@
         <v>2144.5</v>
       </c>
     </row>
-    <row r="3018" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3018" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3018" s="1">
         <v>44750</v>
       </c>
@@ -70328,7 +70324,7 @@
         <v>2146.5</v>
       </c>
     </row>
-    <row r="3019" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3019" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3019" s="1">
         <v>44750</v>
       </c>
@@ -70351,7 +70347,7 @@
         <v>2140.5</v>
       </c>
     </row>
-    <row r="3020" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3020" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3020" s="1">
         <v>44750</v>
       </c>
@@ -70374,7 +70370,7 @@
         <v>2142.5</v>
       </c>
     </row>
-    <row r="3021" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3021" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3021" s="1">
         <v>44750</v>
       </c>
@@ -70397,7 +70393,7 @@
         <v>2132.5</v>
       </c>
     </row>
-    <row r="3022" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3022" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3022" s="1">
         <v>44750</v>
       </c>
@@ -70420,7 +70416,7 @@
         <v>2124.5</v>
       </c>
     </row>
-    <row r="3023" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3023" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3023" s="1">
         <v>44750</v>
       </c>
@@ -70443,7 +70439,7 @@
         <v>2108.5</v>
       </c>
     </row>
-    <row r="3024" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3024" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3024" s="1">
         <v>44750</v>
       </c>
@@ -70466,7 +70462,7 @@
         <v>2140.5</v>
       </c>
     </row>
-    <row r="3025" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3025" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3025" s="1">
         <v>44750</v>
       </c>
@@ -70489,7 +70485,7 @@
         <v>2140.5</v>
       </c>
     </row>
-    <row r="3026" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3026" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3026" s="1">
         <v>44750</v>
       </c>
@@ -70512,7 +70508,7 @@
         <v>2097.5</v>
       </c>
     </row>
-    <row r="3027" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3027" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3027" s="1">
         <v>44750</v>
       </c>
@@ -70535,7 +70531,7 @@
         <v>2093.5</v>
       </c>
     </row>
-    <row r="3028" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3028" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3028" s="1">
         <v>44750</v>
       </c>
@@ -70558,7 +70554,7 @@
         <v>2101.5</v>
       </c>
     </row>
-    <row r="3029" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3029" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3029" s="1">
         <v>44750</v>
       </c>
@@ -70581,7 +70577,7 @@
         <v>2103.5</v>
       </c>
     </row>
-    <row r="3030" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3030" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3030" s="1">
         <v>44750</v>
       </c>
@@ -70604,7 +70600,7 @@
         <v>2203.5</v>
       </c>
     </row>
-    <row r="3031" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3031" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3031" s="1">
         <v>44750</v>
       </c>
@@ -70627,7 +70623,7 @@
         <v>2163.5</v>
       </c>
     </row>
-    <row r="3032" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3032" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3032" s="1">
         <v>44750</v>
       </c>
@@ -70650,7 +70646,7 @@
         <v>2161.5</v>
       </c>
     </row>
-    <row r="3033" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3033" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3033" s="1">
         <v>44750</v>
       </c>
@@ -70673,7 +70669,7 @@
         <v>2157.5</v>
       </c>
     </row>
-    <row r="3034" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3034" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3034" s="1">
         <v>44750</v>
       </c>
@@ -70696,7 +70692,7 @@
         <v>2139.5</v>
       </c>
     </row>
-    <row r="3035" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3035" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3035" s="1">
         <v>44750</v>
       </c>
@@ -70719,7 +70715,7 @@
         <v>2157.5</v>
       </c>
     </row>
-    <row r="3036" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3036" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3036" s="1">
         <v>44750</v>
       </c>
@@ -70742,7 +70738,7 @@
         <v>2157.5</v>
       </c>
     </row>
-    <row r="3037" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3037" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3037" s="1">
         <v>44750</v>
       </c>
@@ -70765,7 +70761,7 @@
         <v>2177.5</v>
       </c>
     </row>
-    <row r="3038" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3038" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3038" s="1">
         <v>44750</v>
       </c>
@@ -70788,7 +70784,7 @@
         <v>2142</v>
       </c>
     </row>
-    <row r="3039" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3039" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3039" s="1">
         <v>44750</v>
       </c>
@@ -70811,7 +70807,7 @@
         <v>2135.1669999999999</v>
       </c>
     </row>
-    <row r="3040" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3040" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3040" s="1">
         <v>44750</v>
       </c>
@@ -70834,7 +70830,7 @@
         <v>2119.1669999999999</v>
       </c>
     </row>
-    <row r="3041" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3041" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3041" s="1">
         <v>44750</v>
       </c>
@@ -70857,7 +70853,7 @@
         <v>2115.1669999999999</v>
       </c>
     </row>
-    <row r="3042" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3042" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3042" s="1">
         <v>44750</v>
       </c>
@@ -70880,7 +70876,7 @@
         <v>2159.8330000000001</v>
       </c>
     </row>
-    <row r="3043" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3043" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3043" s="1">
         <v>44750</v>
       </c>
@@ -70903,7 +70899,7 @@
         <v>2155.8330000000001</v>
       </c>
     </row>
-    <row r="3044" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3044" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3044" s="1">
         <v>44750</v>
       </c>
@@ -70926,7 +70922,7 @@
         <v>2139.8330000000001</v>
       </c>
     </row>
-    <row r="3045" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3045" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3045" s="1">
         <v>44750</v>
       </c>
@@ -70949,7 +70945,7 @@
         <v>2145.1669999999999</v>
       </c>
     </row>
-    <row r="3046" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3046" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3046" s="1">
         <v>44750</v>
       </c>
@@ -70972,7 +70968,7 @@
         <v>2158.8330000000001</v>
       </c>
     </row>
-    <row r="3047" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3047" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3047" s="1">
         <v>44750</v>
       </c>
@@ -70995,7 +70991,7 @@
         <v>2137.5</v>
       </c>
     </row>
-    <row r="3048" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3048" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3048" s="1">
         <v>44750</v>
       </c>
@@ -71018,7 +71014,7 @@
         <v>2128.1669999999999</v>
       </c>
     </row>
-    <row r="3049" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3049" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3049" s="1">
         <v>44750</v>
       </c>
@@ -71041,7 +71037,7 @@
         <v>2138.8330000000001</v>
       </c>
     </row>
-    <row r="3050" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3050" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3050" s="1">
         <v>44750</v>
       </c>
@@ -71064,7 +71060,7 @@
         <v>2151.1669999999999</v>
       </c>
     </row>
-    <row r="3051" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3051" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3051" s="1">
         <v>44750</v>
       </c>
@@ -71087,7 +71083,7 @@
         <v>2123.1669999999999</v>
       </c>
     </row>
-    <row r="3052" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3052" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3052" s="1">
         <v>44750</v>
       </c>
@@ -71110,7 +71106,7 @@
         <v>2119.1669999999999</v>
       </c>
     </row>
-    <row r="3053" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3053" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3053" s="1">
         <v>44750</v>
       </c>
@@ -71133,7 +71129,7 @@
         <v>2113.8330000000001</v>
       </c>
     </row>
-    <row r="3054" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3054" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3054" s="1">
         <v>44750</v>
       </c>
@@ -71156,7 +71152,7 @@
         <v>2116.5</v>
       </c>
     </row>
-    <row r="3055" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3055" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3055" s="1">
         <v>44750</v>
       </c>
@@ -71179,7 +71175,7 @@
         <v>2148.5</v>
       </c>
     </row>
-    <row r="3056" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3056" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3056" s="1">
         <v>44750</v>
       </c>
@@ -71202,7 +71198,7 @@
         <v>2158.5</v>
       </c>
     </row>
-    <row r="3057" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3057" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3057" s="1">
         <v>44750</v>
       </c>
@@ -71225,7 +71221,7 @@
         <v>2152.5</v>
       </c>
     </row>
-    <row r="3058" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3058" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3058" s="1">
         <v>44750</v>
       </c>
@@ -71248,7 +71244,7 @@
         <v>2182.5</v>
       </c>
     </row>
-    <row r="3059" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3059" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3059" s="1">
         <v>44750</v>
       </c>
@@ -71271,7 +71267,7 @@
         <v>2122.5</v>
       </c>
     </row>
-    <row r="3060" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3060" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3060" s="1">
         <v>44750</v>
       </c>
@@ -71294,7 +71290,7 @@
         <v>2126.5</v>
       </c>
     </row>
-    <row r="3061" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3061" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3061" s="1">
         <v>44750</v>
       </c>
@@ -71317,7 +71313,7 @@
         <v>2166.5</v>
       </c>
     </row>
-    <row r="3062" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3062" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3062" s="1">
         <v>44750</v>
       </c>
@@ -71340,7 +71336,7 @@
         <v>2111.8330000000001</v>
       </c>
     </row>
-    <row r="3063" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3063" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3063" s="1">
         <v>44750</v>
       </c>
@@ -71363,7 +71359,7 @@
         <v>2118.5</v>
       </c>
     </row>
-    <row r="3064" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3064" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3064" s="1">
         <v>44750</v>
       </c>
@@ -71386,7 +71382,7 @@
         <v>2149.1669999999999</v>
       </c>
     </row>
-    <row r="3065" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3065" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3065" s="1">
         <v>44750</v>
       </c>
@@ -71409,7 +71405,7 @@
         <v>2159.8330000000001</v>
       </c>
     </row>
-    <row r="3066" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3066" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3066" s="1">
         <v>44750</v>
       </c>
@@ -71432,7 +71428,7 @@
         <v>2101.5</v>
       </c>
     </row>
-    <row r="3067" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3067" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3067" s="1">
         <v>44750</v>
       </c>
@@ -71455,7 +71451,7 @@
         <v>2077.5</v>
       </c>
     </row>
-    <row r="3068" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3068" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3068" s="1">
         <v>44750</v>
       </c>
@@ -71478,7 +71474,7 @@
         <v>2077.5</v>
       </c>
     </row>
-    <row r="3069" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3069" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3069" s="1">
         <v>44750</v>
       </c>
@@ -71501,7 +71497,7 @@
         <v>2098.8330000000001</v>
       </c>
     </row>
-    <row r="3070" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3070" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3070" s="1">
         <v>44750</v>
       </c>
@@ -71524,7 +71520,7 @@
         <v>2108.8330000000001</v>
       </c>
     </row>
-    <row r="3071" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3071" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3071" s="1">
         <v>44750</v>
       </c>
@@ -71547,7 +71543,7 @@
         <v>2080.8330000000001</v>
       </c>
     </row>
-    <row r="3072" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3072" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3072" s="1">
         <v>44750</v>
       </c>
@@ -71570,7 +71566,7 @@
         <v>2072.8330000000001</v>
       </c>
     </row>
-    <row r="3073" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3073" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3073" s="1">
         <v>44750</v>
       </c>
@@ -71593,7 +71589,7 @@
         <v>2144.8330000000001</v>
       </c>
     </row>
-    <row r="3074" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3074" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3074" s="1">
         <v>44750</v>
       </c>
@@ -71616,7 +71612,7 @@
         <v>2226.1669999999999</v>
       </c>
     </row>
-    <row r="3075" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3075" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3075" s="1">
         <v>44750</v>
       </c>
@@ -71639,7 +71635,7 @@
         <v>2198.1669999999999</v>
       </c>
     </row>
-    <row r="3076" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3076" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3076" s="1">
         <v>44750</v>
       </c>
@@ -71662,7 +71658,7 @@
         <v>2186.1669999999999</v>
       </c>
     </row>
-    <row r="3077" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3077" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3077" s="1">
         <v>44750</v>
       </c>
@@ -71685,7 +71681,7 @@
         <v>2168.8330000000001</v>
       </c>
     </row>
-    <row r="3078" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3078" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3078" s="1">
         <v>44750</v>
       </c>
@@ -71708,7 +71704,7 @@
         <v>2137.5</v>
       </c>
     </row>
-    <row r="3079" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3079" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3079" s="1">
         <v>44750</v>
       </c>
@@ -71731,7 +71727,7 @@
         <v>2139.5</v>
       </c>
     </row>
-    <row r="3080" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3080" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3080" s="1">
         <v>44750</v>
       </c>
@@ -71754,7 +71750,7 @@
         <v>2153.5</v>
       </c>
     </row>
-    <row r="3081" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3081" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3081" s="1">
         <v>44750</v>
       </c>
@@ -71777,7 +71773,7 @@
         <v>2179.5</v>
       </c>
     </row>
-    <row r="3082" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3082" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3082" s="1">
         <v>44750</v>
       </c>
@@ -71800,7 +71796,7 @@
         <v>2115.5</v>
       </c>
     </row>
-    <row r="3083" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3083" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3083" s="1">
         <v>44750</v>
       </c>
@@ -71823,7 +71819,7 @@
         <v>2115.5</v>
       </c>
     </row>
-    <row r="3084" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3084" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3084" s="1">
         <v>44750</v>
       </c>
@@ -71846,7 +71842,7 @@
         <v>2107.5</v>
       </c>
     </row>
-    <row r="3085" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3085" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3085" s="1">
         <v>44750</v>
       </c>
@@ -71869,7 +71865,7 @@
         <v>2155.5</v>
       </c>
     </row>
-    <row r="3086" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3086" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3086" s="1">
         <v>44750</v>
       </c>
@@ -71892,7 +71888,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3087" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3087" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3087" s="1">
         <v>44750</v>
       </c>
@@ -71915,7 +71911,7 @@
         <v>2047.5</v>
       </c>
     </row>
-    <row r="3088" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3088" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3088" s="1">
         <v>44750</v>
       </c>
@@ -71938,7 +71934,7 @@
         <v>2043.5</v>
       </c>
     </row>
-    <row r="3089" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3089" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3089" s="1">
         <v>44750</v>
       </c>
@@ -71961,7 +71957,7 @@
         <v>2085.5</v>
       </c>
     </row>
-    <row r="3090" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3090" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3090" s="1">
         <v>44750</v>
       </c>
@@ -71984,7 +71980,7 @@
         <v>2017.5</v>
       </c>
     </row>
-    <row r="3091" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3091" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3091" s="1">
         <v>44750</v>
       </c>
@@ -72007,7 +72003,7 @@
         <v>2011.5</v>
       </c>
     </row>
-    <row r="3092" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3092" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3092" s="1">
         <v>44750</v>
       </c>
@@ -72030,7 +72026,7 @@
         <v>2021.5</v>
       </c>
     </row>
-    <row r="3093" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3093" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3093" s="1">
         <v>44750</v>
       </c>
@@ -78406,6 +78402,7 @@
     <filterColumn colId="0">
       <filters>
         <dateGroupItem year="2022" month="4" dateTimeGrouping="month"/>
+        <dateGroupItem year="2022" month="7" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>